<commit_message>
get abstracts and create wordcloud
</commit_message>
<xml_diff>
--- a/my_google_schoar_stats.xlsx
+++ b/my_google_schoar_stats.xlsx
@@ -396,7 +396,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
@@ -404,7 +404,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
@@ -412,7 +412,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
@@ -420,7 +420,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>